<commit_message>
Exam Center Final commit
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/Examinations.xlsx
+++ b/src/test/resources/ExcelFiles/Examinations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="PROD" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>ExamName</t>
   </si>
@@ -77,9 +77,6 @@
     <t>"Test January 9"</t>
   </si>
   <si>
-    <t>Grade01</t>
-  </si>
-  <si>
     <t>DEC</t>
   </si>
   <si>
@@ -95,38 +92,26 @@
     <t>state</t>
   </si>
   <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Pre Final</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>SmokeTest Jan30</t>
-  </si>
-  <si>
-    <t>Shedule Jan 30</t>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Shedule Jan 31</t>
+  </si>
+  <si>
+    <t>Exam Jan31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,19 +531,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2">
         <v>2024</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>22</v>
@@ -573,10 +558,10 @@
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -588,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,25 +638,25 @@
     </row>
     <row r="2" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2">
         <v>2024</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>22</v>
@@ -686,16 +671,17 @@
         <v>14</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated commit on may 02
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/Examinations.xlsx
+++ b/src/test/resources/ExcelFiles/Examinations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>ExamName</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>SmokeTest Exam mar 06</t>
+  </si>
+  <si>
+    <t>Pipeline Schedule may 02</t>
+  </si>
+  <si>
+    <t>LOC mar 0502</t>
+  </si>
+  <si>
+    <t>SmokeTest Exam may 02</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -559,7 +568,7 @@
       <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="M2" t="s">
@@ -575,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,8 +648,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -652,7 +661,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2">
         <v>2024</v>
@@ -672,8 +681,8 @@
       <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>25</v>
+      <c r="L2" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Updated Modified(Excel files changes) Exam Center Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/Examinations.xlsx
+++ b/src/test/resources/ExcelFiles/Examinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12-ExamCenter/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_17F0BBEFE824839658A587BD4CDADD49BEFC0D3D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B4921E5-7706-4416-9ABB-26CCD15DC8B7}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="11_17F0BBEFE824839658A587BD4CDADD49BEFC0D3D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A2607F5-ABE7-45D4-A77C-3245C756AC60}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>ExamName</t>
   </si>
@@ -69,18 +69,6 @@
     <t>Online Examinations</t>
   </si>
   <si>
-    <t>LocationName</t>
-  </si>
-  <si>
-    <t>AddressField</t>
-  </si>
-  <si>
-    <t>Srinagar colony</t>
-  </si>
-  <si>
-    <t>EditLocationName</t>
-  </si>
-  <si>
     <t>"Test January 9"</t>
   </si>
   <si>
@@ -90,27 +78,15 @@
     <t>Chemistry</t>
   </si>
   <si>
-    <t>Guntur</t>
-  </si>
-  <si>
     <t>"All Questions Test"</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>Smoke Exam oct 2024</t>
   </si>
   <si>
     <t>Smoke Schedule oct 2024</t>
   </si>
   <si>
-    <t>Cambridge12</t>
-  </si>
-  <si>
-    <t>Cambridge13</t>
-  </si>
-  <si>
     <t>Smoke Schedule octa 2024</t>
   </si>
   <si>
@@ -120,13 +96,10 @@
     <t>"Automation test"</t>
   </si>
   <si>
-    <t>Exam Smoke03 2024</t>
-  </si>
-  <si>
-    <t>Schedule Smoke03 2024</t>
-  </si>
-  <si>
-    <t>Canada 01</t>
+    <t>Schedule Smoke06 2024</t>
+  </si>
+  <si>
+    <t>Exam Smoke06 2024</t>
   </si>
 </sst>
 </file>
@@ -148,15 +121,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,21 +143,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,112 +515,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" customWidth="1"/>
-    <col min="11" max="11" width="18.77734375" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="22" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="24.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.109375" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2024</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2024</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -612,10 +617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2464B480-82FB-44D1-8A2C-A2B0FBE8CE3E}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,93 +633,76 @@
     <col min="9" max="9" width="30.44140625" customWidth="1"/>
     <col min="10" max="10" width="17.21875" customWidth="1"/>
     <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="9">
+        <v>2024</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2024</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -724,114 +712,99 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" customWidth="1"/>
-    <col min="11" max="11" width="22.21875" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="29.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="9">
+        <v>2024</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2024</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
+      <c r="L2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>